<commit_message>
"updated liststatus of the character images[3~[C"
</commit_message>
<xml_diff>
--- a/Empire Strikes First/images/Image Checklist.xlsx
+++ b/Empire Strikes First/images/Image Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs_D\Python Games\Empire Strikes First\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26412CB5-4AF6-417B-97E5-C3FAD432FAF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF5B90C-A84D-4E59-A592-10A9B1F87FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39D3D861-168A-4EDD-873B-C17762FC9E69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="28">
   <si>
     <t>Needed Images</t>
   </si>
@@ -178,14 +178,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA44A64B-61D8-460C-9EF1-DB230060BF6B}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,67 +1387,67 @@
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N24" s="4" t="s">
+      <c r="N24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O24" s="4" t="s">
+      <c r="O24" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M25" s="2"/>
-      <c r="N25" s="4" t="s">
+      <c r="N25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O25" s="4" t="s">
+      <c r="O25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M26" s="2"/>
-      <c r="N26" s="4" t="s">
+      <c r="N26" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O26" s="4" t="s">
+      <c r="O26" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M27" s="2"/>
-      <c r="N27" s="4" t="s">
+      <c r="N27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="4" t="s">
+      <c r="O27" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1456,37 +1455,37 @@
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1494,39 +1493,37 @@
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="C35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated status of character images
</commit_message>
<xml_diff>
--- a/Empire Strikes First/images/Image Checklist.xlsx
+++ b/Empire Strikes First/images/Image Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs_D\Python Games\Empire Strikes First\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF5B90C-A84D-4E59-A592-10A9B1F87FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B8CAB0-4E18-48B5-B6A8-F2D73624EFC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39D3D861-168A-4EDD-873B-C17762FC9E69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="28">
   <si>
     <t>Needed Images</t>
   </si>
@@ -1523,7 +1523,9 @@
       <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated character image checklist
</commit_message>
<xml_diff>
--- a/Empire Strikes First/images/Image Checklist.xlsx
+++ b/Empire Strikes First/images/Image Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs_D\Python Games\Empire Strikes First\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B32414-A4D2-4F6A-B9EE-F8B12BD8663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FC7F15-91CD-4B78-9C6A-359FE0912AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39D3D861-168A-4EDD-873B-C17762FC9E69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="28">
   <si>
     <t>Needed Images</t>
   </si>
@@ -1523,7 +1523,9 @@
       <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated character image list to test Github Action
</commit_message>
<xml_diff>
--- a/Empire Strikes First/images/Image Checklist.xlsx
+++ b/Empire Strikes First/images/Image Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs_D\Python Games\Empire Strikes First\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FC7F15-91CD-4B78-9C6A-359FE0912AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB20EE4-18DE-4832-B096-CE59EFB1FC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39D3D861-168A-4EDD-873B-C17762FC9E69}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="29">
   <si>
     <t>Needed Images</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>Drain 1</t>
+  </si>
+  <si>
+    <t>Push 1</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA44A64B-61D8-460C-9EF1-DB230060BF6B}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,6 +1530,36 @@
         <v>18</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A2:C2"/>

</xml_diff>